<commit_message>
filled sheet for default settings.
</commit_message>
<xml_diff>
--- a/Defaultwerte für Parameter.xlsx
+++ b/Defaultwerte für Parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Genomic</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>length of one arm in the hp molecule (from - to)</t>
+  </si>
+  <si>
+    <t>200-500</t>
+  </si>
+  <si>
+    <t>200-400</t>
+  </si>
+  <si>
+    <t>18-25</t>
+  </si>
+  <si>
+    <t>20-32</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>48-60</t>
+  </si>
+  <si>
+    <t>50-200</t>
   </si>
 </sst>
 </file>
@@ -446,16 +467,16 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -489,150 +510,328 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>12</v>
+      </c>
+      <c r="I10" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>30</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
@@ -662,12 +861,24 @@
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>20</v>
       </c>
@@ -679,12 +890,24 @@
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
       <c r="I15" s="1" t="s">
         <v>20</v>
       </c>
@@ -705,9 +928,15 @@
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
       </c>
@@ -723,7 +952,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -735,7 +964,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edited Defaultwerte für Primerparameter
</commit_message>
<xml_diff>
--- a/Defaultwerte für Parameter.xlsx
+++ b/Defaultwerte für Parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Genomic</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>50-200</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -124,12 +127,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -159,10 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,22 +475,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="6" ySplit="17" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -506,268 +520,268 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>10</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>10</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
         <v>6</v>
       </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3">
         <v>6</v>
       </c>
-      <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
         <v>7</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>7</v>
       </c>
-      <c r="H9" s="1">
-        <v>5</v>
-      </c>
-      <c r="I9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>12</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>12</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>12</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>12</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="3">
         <v>12</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -796,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -825,7 +839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -854,7 +868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -883,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -912,7 +926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -939,6 +953,12 @@
       </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -964,7 +984,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned code and deleted files that are not needed
</commit_message>
<xml_diff>
--- a/Defaultwerte für Parameter.xlsx
+++ b/Defaultwerte für Parameter.xlsx
@@ -127,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,12 +174,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -481,7 +488,7 @@
       <pane xSplit="6" ySplit="17" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,7 +639,7 @@
       <c r="H5" s="3">
         <v>3</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -806,7 +813,7 @@
       <c r="H11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -835,7 +842,7 @@
       <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -846,25 +853,25 @@
       <c r="B13" s="1">
         <v>30</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -872,7 +879,7 @@
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1">
@@ -893,7 +900,7 @@
       <c r="H14" s="1">
         <v>3</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -901,7 +908,7 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="1">
@@ -922,7 +929,7 @@
       <c r="H15" s="1">
         <v>3</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -930,28 +937,28 @@
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>